<commit_message>
New formatting sheet, new help text for 2302 and Onwards version.
</commit_message>
<xml_diff>
--- a/VBA_Template_2302_andOnwards/TemplateWithoutVBA.xlsx
+++ b/VBA_Template_2302_andOnwards/TemplateWithoutVBA.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/patrick_weber01_sap_com/Documents/SAP IBP Planning UI/SAP IBP Excel/Planning View Template/2302 v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I519576\Git\VBA_Template_2302_andOnwards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{5BD5591C-06EE-46FB-B401-AEF2D8597221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A394F9A-A3FE-4914-B7A1-9332778115B0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063D5E25-FE55-448D-8B14-5285C8A438AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15345" tabRatio="374" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" tabRatio="374" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SAP IBP Formatting Sheet" sheetId="12" state="hidden" r:id="rId1"/>
+    <sheet name="SAP IBP Formatting Sheet" sheetId="13" state="hidden" r:id="rId1"/>
     <sheet name="Planning View 1" sheetId="5" r:id="rId2"/>
     <sheet name="Planning View 2" sheetId="7" r:id="rId3"/>
   </sheets>
@@ -31,7 +31,9 @@
     <definedName name="DataSecond" localSheetId="0" hidden="1">'SAP IBP Formatting Sheet'!$E$84:$G$84</definedName>
     <definedName name="DataUseFirst" localSheetId="0" hidden="1">'SAP IBP Formatting Sheet'!$H$24</definedName>
     <definedName name="DataUseSecond" localSheetId="0" hidden="1">'SAP IBP Formatting Sheet'!$H$84</definedName>
+    <definedName name="EPMWorkbookOptions_1" localSheetId="0" hidden="1">"IAEAAB+LCAAAAAAAAAqFj7EOgjAURXcT/6HpDgVNHEiBQUcNJgy61vKABmhJWymfLxohUQfX+87Ju5emY9eiAbQRSsY49AOMQHJVCFnF+G5LL9zhNFmv6EXp5qZUk/V2Qg2aPGmi0YgY19b2ESHOOd9tfaUrsgmCkFxPx5zX0DFPSGOZ5IAXq/hv4ekrQnTfAtMHZlkmczZAUrLWACXf8YudO561ssAtFDP9e/jkXYHIc+QCvlcmDz7HneUg"</definedName>
     <definedName name="EPMWorkbookOptions_1" hidden="1">"dgEAAB+LCAAAAAAABACFkMEKgkAQhu9B77DsPVcLOoTaoS5BYhRU10lHXdJZ2d3aHj8pLKpD12++f4b5w/mtqdkVtZGKIh54PmdImcollRG/2GIUTPk8Hg7Cg9Lnk1LntLWdaliXIzO7GRnxytp2JoRzznMTT+lSjH0/EMdkvcsqbGAkyVigDPkrlf9P8e4qY+EWC42mSiltkeICaoOh+IQPb1Ej6CVYSGkHV+zNb/xw+182WlnMLOa9/Tv4"</definedName>
+    <definedName name="EPMWorkbookOptions_2" localSheetId="0" hidden="1">"AQAA"</definedName>
     <definedName name="EPMWorkbookOptions_2" hidden="1">"9F3OxBOtzB60hFONCeryveGHd9WJr+7iO45h/1l2AQAA"</definedName>
     <definedName name="EvenDataFirst" localSheetId="0" hidden="1">'SAP IBP Formatting Sheet'!$F$81</definedName>
     <definedName name="EvenDataSecond" localSheetId="0" hidden="1">'SAP IBP Formatting Sheet'!$F$89</definedName>
@@ -194,7 +196,7 @@
     <author>Weber, Patrick</author>
   </authors>
   <commentList>
-    <comment ref="D40" authorId="0" shapeId="0" xr:uid="{F24AF804-8BC6-4B65-ACF7-A8042E6AC620}">
+    <comment ref="D40" authorId="0" shapeId="0" xr:uid="{854906A5-CD49-4A16-ABAB-A6B02D23F5B3}">
       <text>
         <r>
           <rPr>
@@ -207,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="0" shapeId="0" xr:uid="{26132B1F-514F-4D62-8BEC-044689A9ADFC}">
+    <comment ref="D43" authorId="0" shapeId="0" xr:uid="{35C0CFAA-4700-4D6E-8BD7-D892B6E71F5C}">
       <text>
         <r>
           <rPr>
@@ -220,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D64" authorId="0" shapeId="0" xr:uid="{2060010C-9EED-4580-8ACB-7B83077EE972}">
+    <comment ref="D64" authorId="0" shapeId="0" xr:uid="{0541CBFC-5658-4710-9927-AA79A269FE17}">
       <text>
         <r>
           <rPr>
@@ -233,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D67" authorId="0" shapeId="0" xr:uid="{8AA712B9-46A9-4A62-947B-D4901C945958}">
+    <comment ref="D67" authorId="0" shapeId="0" xr:uid="{8F050922-5F16-4601-9C28-BBB171C9C592}">
       <text>
         <r>
           <rPr>
@@ -365,16 +367,7 @@
     <t>Note: If there are conflicts, the format settings in the lower sections override the ones in the upper section.</t>
   </si>
   <si>
-    <t>In the "10000" and "Label" cells, define the format you want by using the standard Microsoft Office Excel cell formatting functions._x000D_
-Right-click on the cell and define the format settings in the dialog._x000D_
-By default, all the format settings are applied and "All" is displayed in the "Use" column._x000D_
-You can specify which settings of the defined format you want to apply or define additional settings. To do so, double-click in a "Use" cell and define the format settings in the dialog box that opens, or directly enter the format settings in a "Use" cell, using a specific syntax, for example: (FontBold = Y) | (FontSize = 18).</t>
-  </si>
-  <si>
     <t>Member/Property Formatting</t>
-  </si>
-  <si>
-    <t>With these options you can specify which of the formats defined for rows or columns will be applied first if there are conflicts. When you click "Priority to Row", the "Column" section is displayed first in the formatting section, the "Row" section is displayed in second position, and the precedence rules apply.</t>
   </si>
   <si>
     <t>Default Format for Local Member Cells</t>
@@ -390,6 +383,17 @@
   </si>
   <si>
     <t>Day.RELATIVE = 0 OR Week (technical).RELATIVE = 0 OR Week.RELATIVE = 0 OR Month.RELATIVE = 0 OR Quarter.RELATIVE = 0 OR Year.RELATIVE = 0</t>
+  </si>
+  <si>
+    <t>In the cells with the text "10.000" (“Data” column) and "Label" ("Header" columns), you can define the format you want to have in the planning view using the standard Microsoft Excel cell formatting functions.
+For a better overview of the formatting settings, you can right-click the cell and choose "Format Cells…".
+By default, all the formatting settings that have been defined are applied and "All" is displayed in the "Use" column.
+You can further specify which settings (properties) of the defined format you want to be taken over in the planning view. To do so, double-click in a "Use" cell. In the dialog that opens, select the properties you want to use.</t>
+  </si>
+  <si>
+    <t>You can decide if you want the row or the column formatting to overwrite the other by choosing either "Priority to Column" or "Priority to Row" under the header of each section.
+With these options, you can specify whether the formats defined for rows or columns are applied first. For example, when you choose "Priority to Row", the "Column" section is displayed first in the formatting section, and the "Row" section is displayed in second position.
+As the lower rules overwrite the preceding rules, the formatting you define for the "Row" section will be used in the planning view if there are conflicts.</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1038,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1181,6 +1185,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1214,14 +1234,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1239,6 +1251,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1277,26 +1297,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1546,13 +1546,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18433" name="cbApplyLevelFormatting" hidden="1">
+            <xdr:cNvPr id="21505" name="cbApplyLevelFormatting" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18433"/>
+                  <a14:compatExt spid="_x0000_s21505"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E08DBAD-D926-41A3-BA90-178A363D238B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A9855F-5CFE-4952-8738-6A4AD87FAFA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1613,13 +1613,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18434" name="Group Box 2" hidden="1">
+            <xdr:cNvPr id="21506" name="Group Box 2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18434"/>
+                  <a14:compatExt spid="_x0000_s21506"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8AE4B5B-FC1C-4D05-A971-5E7C189D1BA0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1919EDF7-9FE8-45D0-9D6B-33C23334AC24}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1655,7 +1655,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1689,13 +1689,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18435" name="obLevelRowFirst" hidden="1">
+            <xdr:cNvPr id="21507" name="obLevelRowFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18435"/>
+                  <a14:compatExt spid="_x0000_s21507"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8543FD5C-A6EE-4EBD-BEEF-618CAABD39A2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD7D108-6CEC-460B-AECD-79BCF101B2D5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1741,7 +1741,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1775,13 +1775,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18436" name="obLevelColumnFirst" hidden="1">
+            <xdr:cNvPr id="21508" name="obLevelColumnFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18436"/>
+                  <a14:compatExt spid="_x0000_s21508"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{293B3064-4983-4CC2-9A30-D3E3CE4C41C5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05D548AC-3B3D-4F96-8385-1B897A56896C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1827,7 +1827,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1861,13 +1861,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18437" name="cbUseDefaultLevelFirst" hidden="1">
+            <xdr:cNvPr id="21509" name="cbUseDefaultLevelFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18437"/>
+                  <a14:compatExt spid="_x0000_s21509"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FAF8863-9AD8-4D62-8492-704E4DF060D3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D85616-D374-4036-89B6-AE82B9AF3C37}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1913,7 +1913,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1947,13 +1947,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18438" name="cbUseDefaultLevelSecond" hidden="1">
+            <xdr:cNvPr id="21510" name="cbUseDefaultLevelSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18438"/>
+                  <a14:compatExt spid="_x0000_s21510"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEADDBD3-879A-462A-B8AD-4FD51E3D7D16}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D98865F5-B552-4989-B4A7-5EE6AB26CED2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1999,7 +1999,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2033,13 +2033,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18439" name="cbApplyMemberFormatting" hidden="1">
+            <xdr:cNvPr id="21511" name="cbApplyMemberFormatting" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18439"/>
+                  <a14:compatExt spid="_x0000_s21511"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FF11CEC-7CAD-4FD0-8291-A2275569DB0F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E11365-C5AB-44AF-8488-E16890BD07D4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2100,13 +2100,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18440" name="Group Box 8" hidden="1">
+            <xdr:cNvPr id="21512" name="Group Box 8" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18440"/>
+                  <a14:compatExt spid="_x0000_s21512"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA91DE61-88B4-47B8-8299-C67DF8733C14}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCEB7EA-424C-4B69-8044-49ED56479DCD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2142,7 +2142,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2176,13 +2176,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18441" name="obMemberRowFirst" hidden="1">
+            <xdr:cNvPr id="21513" name="obMemberRowFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18441"/>
+                  <a14:compatExt spid="_x0000_s21513"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6303F26-2F4C-476E-A685-A847B3FC7BD0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{499F87E2-B668-46B8-9488-5DD836C3C8BC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2228,7 +2228,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2262,13 +2262,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18442" name="obMemberColumnFirst" hidden="1">
+            <xdr:cNvPr id="21514" name="obMemberColumnFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18442"/>
+                  <a14:compatExt spid="_x0000_s21514"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A7056FB-4D40-47C8-A80E-2B33C333C3DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E395F2-5ED9-4A05-AF92-6A7230BB3060}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2314,7 +2314,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2348,13 +2348,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18443" name="cbApplyCalculatedMemberFirst" hidden="1">
+            <xdr:cNvPr id="21515" name="cbApplyCalculatedMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18443"/>
+                  <a14:compatExt spid="_x0000_s21515"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F9B36D2-FD0B-49FC-B18D-65252D7640A4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87F1F2AB-F9D5-404C-AC1E-290A1613F4C0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2400,7 +2400,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2434,13 +2434,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18444" name="cbApplyImputableMemberFirst" hidden="1">
+            <xdr:cNvPr id="21516" name="cbApplyImputableMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18444"/>
+                  <a14:compatExt spid="_x0000_s21516"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F7961C2-3C9A-4512-AB17-18314F33FC80}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{269F950E-13B0-411D-A1ED-80DCD4DC445E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2486,7 +2486,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2520,13 +2520,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18445" name="cbApplyLocalMemberFirst" hidden="1">
+            <xdr:cNvPr id="21517" name="cbApplyLocalMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18445"/>
+                  <a14:compatExt spid="_x0000_s21517"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688CB9F9-779F-444F-8C11-AE4F351E635B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36E29CEE-5BCC-4D38-80EA-4C665F96075C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2572,7 +2572,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2606,13 +2606,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18446" name="cbApplyChangedMemberFirst" hidden="1">
+            <xdr:cNvPr id="21518" name="cbApplyChangedMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18446"/>
+                  <a14:compatExt spid="_x0000_s21518"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08E69087-75D5-4092-8677-4D166B78D8AE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCF3B8AD-B6A1-4562-928A-F1A0AA0F7DD5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2658,7 +2658,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2692,13 +2692,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18447" name="cbApplySpecificMemberFirst" hidden="1">
+            <xdr:cNvPr id="21519" name="cbApplySpecificMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18447"/>
+                  <a14:compatExt spid="_x0000_s21519"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69279DEE-2B9D-43D3-9418-1D477D37BDDC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31EF6A5A-2913-400D-9007-F46F69896CAC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2744,7 +2744,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2778,13 +2778,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18448" name="AddMemberFirst" hidden="1">
+            <xdr:cNvPr id="21520" name="AddMemberFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18448"/>
+                  <a14:compatExt spid="_x0000_s21520"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F7AA41-AA8A-4AFB-8EFB-F805A11C12FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{308BB146-66BD-4188-B7B3-19B8B6F233BC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2813,7 +2813,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2848,13 +2848,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18449" name="cbApplyCalculatedMemberSecond" hidden="1">
+            <xdr:cNvPr id="21521" name="cbApplyCalculatedMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18449"/>
+                  <a14:compatExt spid="_x0000_s21521"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74577C5F-22D6-42A5-876C-CE86E242E413}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12B60BE8-17C1-4689-A6D3-82DB90387D37}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2900,7 +2900,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2934,13 +2934,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18450" name="cbApplyImputableMemberSecond" hidden="1">
+            <xdr:cNvPr id="21522" name="cbApplyImputableMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18450"/>
+                  <a14:compatExt spid="_x0000_s21522"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BEEF4D4-D3CF-4349-85D2-F350A0FE19D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD238EB-B673-4197-AA81-8393DDE2CB91}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2986,7 +2986,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3020,13 +3020,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18451" name="cbApplyLocalMemberSecond" hidden="1">
+            <xdr:cNvPr id="21523" name="cbApplyLocalMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18451"/>
+                  <a14:compatExt spid="_x0000_s21523"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC879B38-EA8F-4A37-A0B9-6E65FDA4B555}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B464D37C-E808-48F7-93DB-521E30ED6077}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3072,7 +3072,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3106,13 +3106,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18452" name="cbApplyChangedMemberSecond" hidden="1">
+            <xdr:cNvPr id="21524" name="cbApplyChangedMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18452"/>
+                  <a14:compatExt spid="_x0000_s21524"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{746A16A2-5F30-4023-BC23-53CEECB08020}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F96083E-97D4-466F-9C3B-8B833CA25203}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3158,7 +3158,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3192,13 +3192,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18453" name="cbApplySpecificMemberSecond" hidden="1">
+            <xdr:cNvPr id="21525" name="cbApplySpecificMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18453"/>
+                  <a14:compatExt spid="_x0000_s21525"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC0A3A2-1C61-4449-B74A-D09CA344D6EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929DFCED-DB4C-46BD-8BA8-C43DE03B9B77}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3244,7 +3244,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3278,13 +3278,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18454" name="AddMemberSecond" hidden="1">
+            <xdr:cNvPr id="21526" name="AddMemberSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18454"/>
+                  <a14:compatExt spid="_x0000_s21526"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BE97291-1CB7-47A8-9B55-D0AC13FE7B96}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4A5AC71-00A0-45C3-8E12-1C9B71EF7162}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3313,7 +3313,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3348,13 +3348,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18455" name="cbApplyOddEvenFormatting" hidden="1">
+            <xdr:cNvPr id="21527" name="cbApplyOddEvenFormatting" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18455"/>
+                  <a14:compatExt spid="_x0000_s21527"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2324F4AF-A022-45ED-847C-4869A4BEF3DB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0C964B7-6AE7-4F68-A5F3-64CD6737BFAC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3415,13 +3415,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18456" name="Group Box 24" hidden="1">
+            <xdr:cNvPr id="21528" name="Group Box 24" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18456"/>
+                  <a14:compatExt spid="_x0000_s21528"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB43121D-DAC9-4FC2-ADEA-1FDCB86F8127}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5DB70CA-AE90-4FD1-A30E-1118A3DD38F1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3457,7 +3457,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3491,13 +3491,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18457" name="obOddEvenRowFirst" hidden="1">
+            <xdr:cNvPr id="21529" name="obOddEvenRowFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18457"/>
+                  <a14:compatExt spid="_x0000_s21529"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009A377B-6870-4D21-BA18-BB1F78355D19}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6905CA1-30CF-4973-8288-1A03D1BA6BF9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3543,7 +3543,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3577,13 +3577,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18458" name="obOddEvenColumnFirst" hidden="1">
+            <xdr:cNvPr id="21530" name="obOddEvenColumnFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18458"/>
+                  <a14:compatExt spid="_x0000_s21530"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBEE83B9-96E5-48DA-AB44-DC82E9E760C9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191CFB68-A3BA-4424-9E04-10B2CF3B5379}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3629,7 +3629,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3663,13 +3663,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18459" name="cbUseOddFirst" hidden="1">
+            <xdr:cNvPr id="21531" name="cbUseOddFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18459"/>
+                  <a14:compatExt spid="_x0000_s21531"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A04984EA-2D36-418C-A3FC-F7868949AFA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18C8FAC-3C3C-4173-B5FE-766F4762EF37}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3715,7 +3715,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3749,13 +3749,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18460" name="cbUseEvenFirst" hidden="1">
+            <xdr:cNvPr id="21532" name="cbUseEvenFirst" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18460"/>
+                  <a14:compatExt spid="_x0000_s21532"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3E99924-A2DA-4CA1-B0F9-7FA90FEFE46D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5124B558-CB0F-498F-8E70-3B21C140CC31}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3801,7 +3801,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3835,13 +3835,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18461" name="cbUseOddSecond" hidden="1">
+            <xdr:cNvPr id="21533" name="cbUseOddSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18461"/>
+                  <a14:compatExt spid="_x0000_s21533"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6105E24-8F5A-4EB6-A5E5-5CE45CD47840}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0552159-E4AD-4AA0-827D-EC49FE8F5821}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3887,7 +3887,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3921,13 +3921,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18462" name="cbUseEvenSecond" hidden="1">
+            <xdr:cNvPr id="21534" name="cbUseEvenSecond" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18462"/>
+                  <a14:compatExt spid="_x0000_s21534"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{069CEAB7-569A-4FD1-A1E7-6F169BC07F9B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C88A88-693F-438F-81C6-509FEC311D0D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3973,7 +3973,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4007,13 +4007,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18463" name="AddedMember1_1" hidden="1">
+            <xdr:cNvPr id="21535" name="AddedMember1_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18463"/>
+                  <a14:compatExt spid="_x0000_s21535"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7AF9F0A-6E7C-4898-AB94-1C875670B52F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BDE20A7-0C7F-475F-B5CD-4351FA10630E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4042,7 +4042,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4077,13 +4077,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18464" name="ChangeMember1_1" hidden="1">
+            <xdr:cNvPr id="21536" name="ChangeMember1_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18464"/>
+                  <a14:compatExt spid="_x0000_s21536"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55740C13-8F6D-41B3-8D6D-4F028AFCDFCE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD63EEB-1879-4750-866B-B6AC9315B0B8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4112,7 +4112,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4147,13 +4147,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18465" name="UpMember1_1" hidden="1">
+            <xdr:cNvPr id="21537" name="UpMember1_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18465"/>
+                  <a14:compatExt spid="_x0000_s21537"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B0A97BD-52FD-43A6-9409-5446DCCF59B8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0212AC2-DA30-45FC-AE51-82A92433D75C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4182,7 +4182,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4217,13 +4217,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18466" name="DownMember1_1" hidden="1">
+            <xdr:cNvPr id="21538" name="DownMember1_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18466"/>
+                  <a14:compatExt spid="_x0000_s21538"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BDAA045-30EB-4008-9983-7B6182E76A39}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4F8945-A479-49D9-8400-3F37006FF7C6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4252,7 +4252,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4287,13 +4287,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18467" name="AddedMember1_2" hidden="1">
+            <xdr:cNvPr id="21539" name="AddedMember1_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18467"/>
+                  <a14:compatExt spid="_x0000_s21539"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{724ADF45-847F-4657-935B-DCE2E8131A13}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2114FE2A-BBCF-4B2E-8B5A-41DF7A8019CE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4322,7 +4322,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4357,13 +4357,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18468" name="ChangeMember1_2" hidden="1">
+            <xdr:cNvPr id="21540" name="ChangeMember1_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18468"/>
+                  <a14:compatExt spid="_x0000_s21540"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47985356-167A-49C6-9BFF-F3BDED4889CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0D7DFB-338E-4131-BAEB-01CA4216923B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4392,7 +4392,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4427,13 +4427,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18469" name="UpMember1_2" hidden="1">
+            <xdr:cNvPr id="21541" name="UpMember1_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18469"/>
+                  <a14:compatExt spid="_x0000_s21541"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8603DEA-0229-4891-B82B-2A641F6FEFD9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E1DE36-00BA-47C8-8ECF-2AD5171DF88D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4462,7 +4462,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4497,13 +4497,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18470" name="DownMember1_2" hidden="1">
+            <xdr:cNvPr id="21542" name="DownMember1_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18470"/>
+                  <a14:compatExt spid="_x0000_s21542"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCBE0D2B-5B7F-428A-A25A-BC3874A1E162}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F67C77F-269F-4603-ABCF-C4357A0F18CB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4532,7 +4532,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4567,13 +4567,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18471" name="AddedMember2_1" hidden="1">
+            <xdr:cNvPr id="21543" name="AddedMember2_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18471"/>
+                  <a14:compatExt spid="_x0000_s21543"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CF7721-C647-440E-B524-0677334298FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E700FDD3-8C40-441B-9704-68537C485ED1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4602,7 +4602,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4637,13 +4637,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18472" name="ChangeMember2_1" hidden="1">
+            <xdr:cNvPr id="21544" name="ChangeMember2_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18472"/>
+                  <a14:compatExt spid="_x0000_s21544"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DA4867A-A0D5-4EBE-8B9B-B4B0B61D6055}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758E6983-A4EC-4286-A708-3E8B6575598C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4672,7 +4672,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4707,13 +4707,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18473" name="UpMember2_1" hidden="1">
+            <xdr:cNvPr id="21545" name="UpMember2_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18473"/>
+                  <a14:compatExt spid="_x0000_s21545"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF7C3F23-3BE5-4B07-995E-D48178C89FDE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A316BD47-8B00-463B-B9D8-EB4B6E0B5720}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4742,7 +4742,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4777,13 +4777,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18474" name="DownMember2_1" hidden="1">
+            <xdr:cNvPr id="21546" name="DownMember2_1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18474"/>
+                  <a14:compatExt spid="_x0000_s21546"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5F0F75E-2860-4B8F-84BA-00E5BACF073A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A175FE92-01EF-4100-AD6C-6001F92FBD70}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4812,7 +4812,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4847,13 +4847,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18475" name="AddedMember2_2" hidden="1">
+            <xdr:cNvPr id="21547" name="AddedMember2_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18475"/>
+                  <a14:compatExt spid="_x0000_s21547"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B1272D7-6785-49BD-9356-4AE71215FCBA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E318D8-D8EE-4E20-A3CD-979B68ED5AF4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4882,7 +4882,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4917,13 +4917,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18476" name="ChangeMember2_2" hidden="1">
+            <xdr:cNvPr id="21548" name="ChangeMember2_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18476"/>
+                  <a14:compatExt spid="_x0000_s21548"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{573C9CA0-EA45-4FF3-972A-3247AF5B9CE9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6873446-673D-431B-82D3-4400D4BC80E1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4952,7 +4952,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4987,13 +4987,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18477" name="UpMember2_2" hidden="1">
+            <xdr:cNvPr id="21549" name="UpMember2_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18477"/>
+                  <a14:compatExt spid="_x0000_s21549"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AB13180-F236-4804-96E7-50B34E5AAD70}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1D968B5-007F-4294-8CD1-FCA069B9C104}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5022,7 +5022,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5057,13 +5057,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18478" name="DownMember2_2" hidden="1">
+            <xdr:cNvPr id="21550" name="DownMember2_2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s18478"/>
+                  <a14:compatExt spid="_x0000_s21550"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B560BAFA-CDA2-4DE4-947A-D54EDB000074}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A9F10F8-AB4C-4959-A5FA-41AB879E4C57}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5092,7 +5092,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -5713,15 +5713,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC8CFAB-36D8-4609-B4B9-DA61B9EBB6A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B77CAB-315F-4159-B8FE-5F3222B13478}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Q146"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
@@ -5744,19 +5744,19 @@
   <sheetData>
     <row r="1" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
@@ -5806,43 +5806,43 @@
     </row>
     <row r="5" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="74"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="78"/>
       <c r="Q5" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="77"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
       <c r="Q6" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="15"/>
@@ -5855,13 +5855,13 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="16"/>
-      <c r="Q7" s="70" t="s">
-        <v>30</v>
+      <c r="Q7" s="74" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="53"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5872,35 +5872,35 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="10"/>
-      <c r="Q8" s="70"/>
+      <c r="Q8" s="74"/>
     </row>
     <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="53"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="56"/>
-      <c r="K9" s="57"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="61"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="70"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="2"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
@@ -5910,12 +5910,12 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="10"/>
-      <c r="Q10" s="70"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="35" t="s">
         <v>8</v>
       </c>
@@ -5935,12 +5935,12 @@
       <c r="L11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="70"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="61"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="13"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -5950,11 +5950,11 @@
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="14"/>
-      <c r="Q12" s="70"/>
+      <c r="Q12" s="74"/>
     </row>
     <row r="13" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2"/>
@@ -5967,11 +5967,11 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="10"/>
-      <c r="Q13" s="70"/>
+      <c r="Q13" s="74"/>
     </row>
     <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -5982,35 +5982,35 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="10"/>
-      <c r="Q14" s="70"/>
+      <c r="Q14" s="74"/>
     </row>
     <row r="15" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="53"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
       <c r="H15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="56"/>
-      <c r="K15" s="57"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="61"/>
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="70"/>
+      <c r="Q15" s="74"/>
     </row>
     <row r="16" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="2"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
@@ -6020,12 +6020,12 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="10"/>
-      <c r="Q16" s="70"/>
+      <c r="Q16" s="74"/>
     </row>
     <row r="17" spans="1:17" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="35" t="s">
         <v>8</v>
       </c>
@@ -6045,12 +6045,12 @@
       <c r="L17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="70"/>
+      <c r="Q17" s="74"/>
     </row>
     <row r="18" spans="1:17" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="61"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="13"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -6060,7 +6060,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="14"/>
-      <c r="Q18" s="70"/>
+      <c r="Q18" s="74"/>
     </row>
     <row r="19" spans="1:17" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
@@ -6075,7 +6075,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="Q19" s="70"/>
+      <c r="Q19" s="74"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
@@ -6094,43 +6094,43 @@
     </row>
     <row r="21" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="66"/>
+      <c r="B21" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="68"/>
       <c r="Q21" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="69"/>
-      <c r="Q22" s="70" t="s">
-        <v>32</v>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="71"/>
+      <c r="Q22" s="74" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2"/>
@@ -6143,35 +6143,35 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="10"/>
-      <c r="Q23" s="70"/>
+      <c r="Q23" s="74"/>
     </row>
     <row r="24" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="53"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="61"/>
       <c r="H24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="55" t="s">
+      <c r="I24" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J24" s="56"/>
-      <c r="K24" s="57"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="61"/>
       <c r="L24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="70"/>
+      <c r="Q24" s="74"/>
     </row>
     <row r="25" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="58"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="2"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
@@ -6181,17 +6181,17 @@
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="10"/>
-      <c r="Q25" s="70"/>
+      <c r="Q25" s="74"/>
     </row>
     <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="34"/>
-      <c r="F26" s="81">
+      <c r="F26" s="52">
         <v>10000</v>
       </c>
       <c r="G26" s="34"/>
@@ -6206,12 +6206,12 @@
       <c r="L26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q26" s="70"/>
+      <c r="Q26" s="74"/>
     </row>
     <row r="27" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="60"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="50"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -6221,12 +6221,12 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="51"/>
-      <c r="Q27" s="70"/>
+      <c r="Q27" s="74"/>
     </row>
     <row r="28" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="59"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="2"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
@@ -6236,12 +6236,12 @@
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
       <c r="L28" s="10"/>
-      <c r="Q28" s="70"/>
+      <c r="Q28" s="74"/>
     </row>
     <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="59"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="63"/>
       <c r="D29" s="35" t="s">
         <v>15</v>
       </c>
@@ -6261,12 +6261,12 @@
       <c r="L29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q29" s="70"/>
+      <c r="Q29" s="74"/>
     </row>
     <row r="30" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="60"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="64"/>
       <c r="D30" s="50"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -6280,8 +6280,8 @@
     </row>
     <row r="31" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="59"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="2"/>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
@@ -6294,13 +6294,13 @@
     </row>
     <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="59"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="63"/>
       <c r="D32" s="35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E32" s="34"/>
-      <c r="F32" s="81">
+      <c r="F32" s="52">
         <v>10000</v>
       </c>
       <c r="G32" s="34"/>
@@ -6318,8 +6318,8 @@
     </row>
     <row r="33" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="60"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="50"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -6332,8 +6332,8 @@
     </row>
     <row r="34" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="59"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="63"/>
       <c r="D34" s="2"/>
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
@@ -6346,10 +6346,10 @@
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="59"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="34"/>
       <c r="F35" s="44">
@@ -6370,8 +6370,8 @@
     </row>
     <row r="36" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="60"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="50"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -6384,8 +6384,8 @@
     </row>
     <row r="37" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="59"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="63"/>
       <c r="D37" s="2"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -6398,8 +6398,8 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="59"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="63"/>
       <c r="D38" s="35" t="s">
         <v>17</v>
       </c>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="39" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="53"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="48"/>
       <c r="D39" s="35"/>
       <c r="E39" s="34"/>
@@ -6428,13 +6428,13 @@
     </row>
     <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="53"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="48"/>
       <c r="D40" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="34"/>
-      <c r="F40" s="82">
+      <c r="F40" s="53">
         <v>10000</v>
       </c>
       <c r="G40" s="34"/>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="41" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="53"/>
+      <c r="B41" s="57"/>
       <c r="C41" s="48"/>
       <c r="D41" s="31"/>
       <c r="E41" s="7"/>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="42" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="53"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="48"/>
       <c r="D42" s="35"/>
       <c r="E42" s="34"/>
@@ -6478,15 +6478,15 @@
       <c r="K42" s="34"/>
       <c r="L42" s="10"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="53"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="48"/>
       <c r="D43" s="40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E43" s="34"/>
-      <c r="F43" s="83">
+      <c r="F43" s="54">
         <v>1</v>
       </c>
       <c r="G43" s="34"/>
@@ -6494,7 +6494,7 @@
         <v>27</v>
       </c>
       <c r="I43" s="34"/>
-      <c r="J43" s="84" t="s">
+      <c r="J43" s="38" t="s">
         <v>10</v>
       </c>
       <c r="K43" s="34"/>
@@ -6504,7 +6504,7 @@
     </row>
     <row r="44" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="53"/>
+      <c r="B44" s="57"/>
       <c r="C44" s="48"/>
       <c r="D44" s="31"/>
       <c r="E44" s="7"/>
@@ -6518,7 +6518,7 @@
     </row>
     <row r="45" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="53"/>
+      <c r="B45" s="57"/>
       <c r="C45" s="48"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="46" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="54"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="49"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
@@ -6546,7 +6546,7 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="15"/>
@@ -6562,30 +6562,30 @@
     </row>
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
-      <c r="B48" s="53"/>
+      <c r="B48" s="57"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="55" t="s">
+      <c r="E48" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="57"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="61"/>
       <c r="H48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I48" s="55" t="s">
+      <c r="I48" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="56"/>
-      <c r="K48" s="57"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="61"/>
       <c r="L48" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="58"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="62"/>
       <c r="D49" s="2"/>
       <c r="E49" s="34"/>
       <c r="F49" s="34"/>
@@ -6598,13 +6598,13 @@
     </row>
     <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="59"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="63"/>
       <c r="D50" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="34"/>
-      <c r="F50" s="81">
+      <c r="F50" s="52">
         <v>10000</v>
       </c>
       <c r="G50" s="34"/>
@@ -6622,8 +6622,8 @@
     </row>
     <row r="51" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="60"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="50"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -6636,8 +6636,8 @@
     </row>
     <row r="52" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="59"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="2"/>
       <c r="E52" s="34"/>
       <c r="F52" s="34"/>
@@ -6650,13 +6650,13 @@
     </row>
     <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="59"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="63"/>
       <c r="D53" s="35" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="34"/>
-      <c r="F53" s="81">
+      <c r="F53" s="52">
         <v>10000</v>
       </c>
       <c r="G53" s="34"/>
@@ -6674,8 +6674,8 @@
     </row>
     <row r="54" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="60"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="64"/>
       <c r="D54" s="50"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -6688,8 +6688,8 @@
     </row>
     <row r="55" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="59"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="2"/>
       <c r="E55" s="34"/>
       <c r="F55" s="34"/>
@@ -6702,13 +6702,13 @@
     </row>
     <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="59"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E56" s="34"/>
-      <c r="F56" s="81">
+      <c r="F56" s="52">
         <v>10000</v>
       </c>
       <c r="G56" s="34"/>
@@ -6726,8 +6726,8 @@
     </row>
     <row r="57" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="60"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="64"/>
       <c r="D57" s="50"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -6740,8 +6740,8 @@
     </row>
     <row r="58" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="59"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="63"/>
       <c r="D58" s="2"/>
       <c r="E58" s="34"/>
       <c r="F58" s="34"/>
@@ -6754,13 +6754,13 @@
     </row>
     <row r="59" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="59"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="63"/>
       <c r="D59" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E59" s="34"/>
-      <c r="F59" s="81">
+      <c r="F59" s="52">
         <v>10000</v>
       </c>
       <c r="G59" s="34"/>
@@ -6778,8 +6778,8 @@
     </row>
     <row r="60" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="60"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="64"/>
       <c r="D60" s="50"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -6792,8 +6792,8 @@
     </row>
     <row r="61" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="59"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="63"/>
       <c r="D61" s="2"/>
       <c r="E61" s="34"/>
       <c r="F61" s="34"/>
@@ -6806,8 +6806,8 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
-      <c r="B62" s="53"/>
-      <c r="C62" s="59"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="63"/>
       <c r="D62" s="35" t="s">
         <v>17</v>
       </c>
@@ -6822,7 +6822,7 @@
     </row>
     <row r="63" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
-      <c r="B63" s="53"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="48"/>
       <c r="D63" s="35"/>
       <c r="E63" s="34"/>
@@ -6836,13 +6836,13 @@
     </row>
     <row r="64" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
-      <c r="B64" s="53"/>
+      <c r="B64" s="57"/>
       <c r="C64" s="48"/>
       <c r="D64" s="40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E64" s="34"/>
-      <c r="F64" s="85">
+      <c r="F64" s="55">
         <v>10000</v>
       </c>
       <c r="G64" s="34"/>
@@ -6850,7 +6850,7 @@
         <v>19</v>
       </c>
       <c r="I64" s="34"/>
-      <c r="J64" s="84" t="s">
+      <c r="J64" s="38" t="s">
         <v>10</v>
       </c>
       <c r="K64" s="34"/>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="65" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
-      <c r="B65" s="53"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="48"/>
       <c r="D65" s="31"/>
       <c r="E65" s="7"/>
@@ -6874,7 +6874,7 @@
     </row>
     <row r="66" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
-      <c r="B66" s="53"/>
+      <c r="B66" s="57"/>
       <c r="C66" s="48"/>
       <c r="D66" s="35"/>
       <c r="E66" s="34"/>
@@ -6888,13 +6888,13 @@
     </row>
     <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
-      <c r="B67" s="53"/>
+      <c r="B67" s="57"/>
       <c r="C67" s="48"/>
       <c r="D67" s="40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E67" s="34"/>
-      <c r="F67" s="81">
+      <c r="F67" s="52">
         <v>10000</v>
       </c>
       <c r="G67" s="34"/>
@@ -6912,7 +6912,7 @@
     </row>
     <row r="68" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
-      <c r="B68" s="53"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="48"/>
       <c r="D68" s="31"/>
       <c r="E68" s="7"/>
@@ -6926,7 +6926,7 @@
     </row>
     <row r="69" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="53"/>
+      <c r="B69" s="57"/>
       <c r="C69" s="48"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="70" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-      <c r="B70" s="54"/>
+      <c r="B70" s="58"/>
       <c r="C70" s="49"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
@@ -6982,37 +6982,37 @@
     </row>
     <row r="73" spans="1:12" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
-      <c r="B73" s="64" t="s">
+      <c r="B73" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
-      <c r="K73" s="65"/>
-      <c r="L73" s="66"/>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="67"/>
+      <c r="H73" s="67"/>
+      <c r="I73" s="67"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="67"/>
+      <c r="L73" s="68"/>
     </row>
     <row r="74" spans="1:12" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
-      <c r="B74" s="67"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="68"/>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="69"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="70"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="I74" s="70"/>
+      <c r="J74" s="70"/>
+      <c r="K74" s="70"/>
+      <c r="L74" s="71"/>
     </row>
     <row r="75" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
-      <c r="B75" s="52" t="s">
+      <c r="B75" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C75" s="2"/>
@@ -7028,30 +7028,30 @@
     </row>
     <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
-      <c r="B76" s="53"/>
+      <c r="B76" s="57"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
-      <c r="E76" s="55" t="s">
+      <c r="E76" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="56"/>
-      <c r="G76" s="57"/>
+      <c r="F76" s="60"/>
+      <c r="G76" s="61"/>
       <c r="H76" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I76" s="55" t="s">
+      <c r="I76" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J76" s="56"/>
-      <c r="K76" s="57"/>
+      <c r="J76" s="60"/>
+      <c r="K76" s="61"/>
       <c r="L76" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
-      <c r="B77" s="53"/>
-      <c r="C77" s="58"/>
+      <c r="B77" s="57"/>
+      <c r="C77" s="62"/>
       <c r="D77" s="2"/>
       <c r="E77" s="34"/>
       <c r="F77" s="34"/>
@@ -7064,13 +7064,13 @@
     </row>
     <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
-      <c r="B78" s="53"/>
-      <c r="C78" s="59"/>
+      <c r="B78" s="57"/>
+      <c r="C78" s="63"/>
       <c r="D78" s="35" t="s">
         <v>21</v>
       </c>
       <c r="E78" s="34"/>
-      <c r="F78" s="81">
+      <c r="F78" s="52">
         <v>10000</v>
       </c>
       <c r="G78" s="34"/>
@@ -7088,8 +7088,8 @@
     </row>
     <row r="79" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="60"/>
+      <c r="B79" s="57"/>
+      <c r="C79" s="64"/>
       <c r="D79" s="50"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
@@ -7102,8 +7102,8 @@
     </row>
     <row r="80" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
-      <c r="B80" s="53"/>
-      <c r="C80" s="59"/>
+      <c r="B80" s="57"/>
+      <c r="C80" s="63"/>
       <c r="D80" s="2"/>
       <c r="E80" s="34"/>
       <c r="F80" s="34"/>
@@ -7116,13 +7116,13 @@
     </row>
     <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
-      <c r="B81" s="53"/>
-      <c r="C81" s="59"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="63"/>
       <c r="D81" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E81" s="34"/>
-      <c r="F81" s="81">
+      <c r="F81" s="52">
         <v>10000</v>
       </c>
       <c r="G81" s="34"/>
@@ -7140,8 +7140,8 @@
     </row>
     <row r="82" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
-      <c r="B82" s="62"/>
-      <c r="C82" s="60"/>
+      <c r="B82" s="72"/>
+      <c r="C82" s="64"/>
       <c r="D82" s="50"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="83" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
-      <c r="B83" s="52" t="s">
+      <c r="B83" s="56" t="s">
         <v>4</v>
       </c>
       <c r="C83" s="2"/>
@@ -7170,30 +7170,30 @@
     </row>
     <row r="84" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
-      <c r="B84" s="53"/>
+      <c r="B84" s="57"/>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
-      <c r="E84" s="55" t="s">
+      <c r="E84" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="56"/>
-      <c r="G84" s="57"/>
+      <c r="F84" s="60"/>
+      <c r="G84" s="61"/>
       <c r="H84" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I84" s="55" t="s">
+      <c r="I84" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J84" s="56"/>
-      <c r="K84" s="57"/>
+      <c r="J84" s="60"/>
+      <c r="K84" s="61"/>
       <c r="L84" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
-      <c r="B85" s="53"/>
-      <c r="C85" s="58"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="62"/>
       <c r="D85" s="2"/>
       <c r="E85" s="34"/>
       <c r="F85" s="34"/>
@@ -7206,13 +7206,13 @@
     </row>
     <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
-      <c r="B86" s="53"/>
-      <c r="C86" s="59"/>
+      <c r="B86" s="57"/>
+      <c r="C86" s="63"/>
       <c r="D86" s="35" t="s">
         <v>21</v>
       </c>
       <c r="E86" s="34"/>
-      <c r="F86" s="81">
+      <c r="F86" s="52">
         <v>10000</v>
       </c>
       <c r="G86" s="34"/>
@@ -7230,8 +7230,8 @@
     </row>
     <row r="87" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
-      <c r="B87" s="53"/>
-      <c r="C87" s="60"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="64"/>
       <c r="D87" s="50"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -7244,8 +7244,8 @@
     </row>
     <row r="88" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
-      <c r="B88" s="53"/>
-      <c r="C88" s="59"/>
+      <c r="B88" s="57"/>
+      <c r="C88" s="63"/>
       <c r="D88" s="2"/>
       <c r="E88" s="34"/>
       <c r="F88" s="34"/>
@@ -7258,13 +7258,13 @@
     </row>
     <row r="89" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
-      <c r="B89" s="53"/>
-      <c r="C89" s="59"/>
+      <c r="B89" s="57"/>
+      <c r="C89" s="63"/>
       <c r="D89" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E89" s="34"/>
-      <c r="F89" s="81">
+      <c r="F89" s="52">
         <v>10000</v>
       </c>
       <c r="G89" s="34"/>
@@ -7282,8 +7282,8 @@
     </row>
     <row r="90" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
-      <c r="B90" s="54"/>
-      <c r="C90" s="61"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="65"/>
       <c r="D90" s="13"/>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -8132,7 +8132,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18455" r:id="rId4" name="cbApplyOddEvenFormatting">
+        <control shapeId="21527" r:id="rId4" name="cbApplyOddEvenFormatting">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -8152,12 +8152,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="18455" r:id="rId4" name="cbApplyOddEvenFormatting"/>
+        <control shapeId="21527" r:id="rId4" name="cbApplyOddEvenFormatting"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18439" r:id="rId6" name="cbApplyMemberFormatting">
+        <control shapeId="21511" r:id="rId6" name="cbApplyMemberFormatting">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
@@ -8177,12 +8177,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="18439" r:id="rId6" name="cbApplyMemberFormatting"/>
+        <control shapeId="21511" r:id="rId6" name="cbApplyMemberFormatting"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18433" r:id="rId8" name="cbApplyLevelFormatting">
+        <control shapeId="21505" r:id="rId8" name="cbApplyLevelFormatting">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
@@ -8202,12 +8202,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="18433" r:id="rId8" name="cbApplyLevelFormatting"/>
+        <control shapeId="21505" r:id="rId8" name="cbApplyLevelFormatting"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18434" r:id="rId10" name="Group Box 2">
+        <control shapeId="21506" r:id="rId10" name="Group Box 2">
           <controlPr defaultSize="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8229,7 +8229,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18435" r:id="rId11" name="obLevelRowFirst">
+        <control shapeId="21507" r:id="rId11" name="obLevelRowFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8251,7 +8251,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18436" r:id="rId12" name="obLevelColumnFirst">
+        <control shapeId="21508" r:id="rId12" name="obLevelColumnFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8273,7 +8273,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18437" r:id="rId13" name="cbUseDefaultLevelFirst">
+        <control shapeId="21509" r:id="rId13" name="cbUseDefaultLevelFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8295,7 +8295,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18438" r:id="rId14" name="cbUseDefaultLevelSecond">
+        <control shapeId="21510" r:id="rId14" name="cbUseDefaultLevelSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8317,7 +8317,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18440" r:id="rId15" name="Group Box 8">
+        <control shapeId="21512" r:id="rId15" name="Group Box 8">
           <controlPr defaultSize="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8339,7 +8339,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18441" r:id="rId16" name="obMemberRowFirst">
+        <control shapeId="21513" r:id="rId16" name="obMemberRowFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8361,7 +8361,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18442" r:id="rId17" name="obMemberColumnFirst">
+        <control shapeId="21514" r:id="rId17" name="obMemberColumnFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8383,7 +8383,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18443" r:id="rId18" name="cbApplyCalculatedMemberFirst">
+        <control shapeId="21515" r:id="rId18" name="cbApplyCalculatedMemberFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8405,7 +8405,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18444" r:id="rId19" name="cbApplyImputableMemberFirst">
+        <control shapeId="21516" r:id="rId19" name="cbApplyImputableMemberFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8427,7 +8427,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18445" r:id="rId20" name="cbApplyLocalMemberFirst">
+        <control shapeId="21517" r:id="rId20" name="cbApplyLocalMemberFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8449,7 +8449,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18446" r:id="rId21" name="cbApplyChangedMemberFirst">
+        <control shapeId="21518" r:id="rId21" name="cbApplyChangedMemberFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8471,7 +8471,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18447" r:id="rId22" name="cbApplySpecificMemberFirst">
+        <control shapeId="21519" r:id="rId22" name="cbApplySpecificMemberFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8493,7 +8493,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18448" r:id="rId23" name="AddMemberFirst">
+        <control shapeId="21520" r:id="rId23" name="AddMemberFirst">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8515,7 +8515,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18449" r:id="rId24" name="cbApplyCalculatedMemberSecond">
+        <control shapeId="21521" r:id="rId24" name="cbApplyCalculatedMemberSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8537,7 +8537,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18450" r:id="rId25" name="cbApplyImputableMemberSecond">
+        <control shapeId="21522" r:id="rId25" name="cbApplyImputableMemberSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8559,7 +8559,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18451" r:id="rId26" name="cbApplyLocalMemberSecond">
+        <control shapeId="21523" r:id="rId26" name="cbApplyLocalMemberSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8581,7 +8581,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18452" r:id="rId27" name="cbApplyChangedMemberSecond">
+        <control shapeId="21524" r:id="rId27" name="cbApplyChangedMemberSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8603,7 +8603,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18453" r:id="rId28" name="cbApplySpecificMemberSecond">
+        <control shapeId="21525" r:id="rId28" name="cbApplySpecificMemberSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8625,7 +8625,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18454" r:id="rId29" name="AddMemberSecond">
+        <control shapeId="21526" r:id="rId29" name="AddMemberSecond">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8647,7 +8647,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18456" r:id="rId30" name="Group Box 24">
+        <control shapeId="21528" r:id="rId30" name="Group Box 24">
           <controlPr defaultSize="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8669,7 +8669,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18457" r:id="rId31" name="obOddEvenRowFirst">
+        <control shapeId="21529" r:id="rId31" name="obOddEvenRowFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8691,7 +8691,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18458" r:id="rId32" name="obOddEvenColumnFirst">
+        <control shapeId="21530" r:id="rId32" name="obOddEvenColumnFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1">
               <from>
@@ -8713,7 +8713,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18459" r:id="rId33" name="cbUseOddFirst">
+        <control shapeId="21531" r:id="rId33" name="cbUseOddFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8735,7 +8735,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18460" r:id="rId34" name="cbUseEvenFirst">
+        <control shapeId="21532" r:id="rId34" name="cbUseEvenFirst">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8757,7 +8757,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18461" r:id="rId35" name="cbUseOddSecond">
+        <control shapeId="21533" r:id="rId35" name="cbUseOddSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8779,7 +8779,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18462" r:id="rId36" name="cbUseEvenSecond">
+        <control shapeId="21534" r:id="rId36" name="cbUseEvenSecond">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
             <anchor moveWithCells="1">
               <from>
@@ -8801,7 +8801,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18463" r:id="rId37" name="AddedMember1_1">
+        <control shapeId="21535" r:id="rId37" name="AddedMember1_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8823,7 +8823,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18464" r:id="rId38" name="ChangeMember1_1">
+        <control shapeId="21536" r:id="rId38" name="ChangeMember1_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8845,7 +8845,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18465" r:id="rId39" name="UpMember1_1">
+        <control shapeId="21537" r:id="rId39" name="UpMember1_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8867,7 +8867,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18466" r:id="rId40" name="DownMember1_1">
+        <control shapeId="21538" r:id="rId40" name="DownMember1_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8889,7 +8889,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18467" r:id="rId41" name="AddedMember1_2">
+        <control shapeId="21539" r:id="rId41" name="AddedMember1_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8911,7 +8911,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18468" r:id="rId42" name="ChangeMember1_2">
+        <control shapeId="21540" r:id="rId42" name="ChangeMember1_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8933,7 +8933,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18469" r:id="rId43" name="UpMember1_2">
+        <control shapeId="21541" r:id="rId43" name="UpMember1_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8955,7 +8955,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18470" r:id="rId44" name="DownMember1_2">
+        <control shapeId="21542" r:id="rId44" name="DownMember1_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8977,7 +8977,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18471" r:id="rId45" name="AddedMember2_1">
+        <control shapeId="21543" r:id="rId45" name="AddedMember2_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -8999,7 +8999,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18472" r:id="rId46" name="ChangeMember2_1">
+        <control shapeId="21544" r:id="rId46" name="ChangeMember2_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9021,7 +9021,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18473" r:id="rId47" name="UpMember2_1">
+        <control shapeId="21545" r:id="rId47" name="UpMember2_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9043,7 +9043,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18474" r:id="rId48" name="DownMember2_1">
+        <control shapeId="21546" r:id="rId48" name="DownMember2_1">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9065,7 +9065,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18475" r:id="rId49" name="AddedMember2_2">
+        <control shapeId="21547" r:id="rId49" name="AddedMember2_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9087,7 +9087,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18476" r:id="rId50" name="ChangeMember2_2">
+        <control shapeId="21548" r:id="rId50" name="ChangeMember2_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9109,7 +9109,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18477" r:id="rId51" name="UpMember2_2">
+        <control shapeId="21549" r:id="rId51" name="UpMember2_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9131,7 +9131,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="18478" r:id="rId52" name="DownMember2_2">
+        <control shapeId="21550" r:id="rId52" name="DownMember2_2">
           <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.IBPXLClient.TechnicalCategory.ButtonActionInIBPClientFormattingSheet">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -9176,19 +9176,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="str">
+      <c r="A1" s="82" t="str">
         <f>" IBP | " &amp;IFERROR(IF(SOP_Favorite_Name&lt;&gt;" ",SOP_Favorite_Name,IF(SOP_Template_Name&lt;&gt;" ",SOP_Template_Name,"Ad Hoc Planning View")),"Offline")</f>
         <v xml:space="preserve"> IBP | Ad Hoc Planning View</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
       <c r="M1" s="43"/>
@@ -9234,19 +9234,19 @@
       <c r="CG1" s="27"/>
     </row>
     <row r="2" spans="1:85" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="str">
-        <f>"Planning Area: "&amp;IFERROR(_xlfn.SINGLE(SOP_Planning_Area),"Offline")&amp;" | User: "&amp;_xlfn.SINGLE(_xll.IBPUser())</f>
-        <v>Planning Area: PLAIBP1 | User: #Error, no current connection.</v>
-      </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+      <c r="A2" s="84" t="e">
+        <f ca="1">"Planning Area: "&amp;IFERROR(_xlfn.SINGLE(SOP_Planning_Area),"Offline")&amp;" | User: "&amp;_xlfn.SINGLE(_xll.IBPUser())</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="43"/>
       <c r="L2" s="43"/>
       <c r="M2" s="43"/>
@@ -9292,19 +9292,19 @@
       <c r="CG2" s="27"/>
     </row>
     <row r="3" spans="1:85" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="str" cm="1">
+      <c r="A3" s="84" t="str" cm="1">
         <f t="array" ref="A3">"Last Refresh: "&amp;IFERROR(YEAR(SOP_Refresh_Timestamp)&amp;"-"&amp;TEXT(SOP_Refresh_Timestamp,"MMM")&amp;"-"&amp;DAY(SOP_Refresh_Timestamp)&amp;" "&amp;TEXT(SOP_Refresh_Timestamp,"HH:MM:SS"),"Offline")&amp;" | UoM: "&amp;IFERROR(SOP_TargetUoM,"(None)")&amp;" | Currency: "&amp;IFERROR(SOP_TargetCurrency,"(None)")</f>
         <v>Last Refresh: 1900-Jan-0 00:00:00 | UoM: (None) | Currency: (None)</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
       <c r="M3" s="43"/>
@@ -9538,19 +9538,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="str">
+      <c r="A1" s="82" t="str">
         <f>" IBP | " &amp;IFERROR(IF(SOP_Favorite_Name&lt;&gt;" ",SOP_Favorite_Name,IF(SOP_Template_Name&lt;&gt;" ",SOP_Template_Name,"Ad Hoc Planning View")),"Offline")</f>
         <v xml:space="preserve"> IBP | Ad Hoc Planning View</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
       <c r="K1" s="42"/>
       <c r="L1" s="42"/>
       <c r="M1" s="42"/>
@@ -9596,19 +9596,19 @@
       <c r="CG1" s="27"/>
     </row>
     <row r="2" spans="1:85" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="str">
-        <f>"Planning Area: "&amp;IFERROR(_xlfn.SINGLE(SOP_Planning_Area),"Offline")&amp;" | User: "&amp;_xlfn.SINGLE(_xll.IBPUser())</f>
-        <v>Planning Area: PLAIBP1 | User: #Error, no current connection.</v>
-      </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+      <c r="A2" s="84" t="e">
+        <f ca="1">"Planning Area: "&amp;IFERROR(_xlfn.SINGLE(SOP_Planning_Area),"Offline")&amp;" | User: "&amp;_xlfn.SINGLE(_xll.IBPUser())</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="42"/>
       <c r="L2" s="42"/>
       <c r="M2" s="42"/>
@@ -9654,19 +9654,19 @@
       <c r="CG2" s="27"/>
     </row>
     <row r="3" spans="1:85" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="str" cm="1">
+      <c r="A3" s="84" t="str" cm="1">
         <f t="array" ref="A3">"Last Refresh: "&amp;IFERROR(YEAR(SOP_Refresh_Timestamp)&amp;"-"&amp;TEXT(SOP_Refresh_Timestamp,"MMM")&amp;"-"&amp;DAY(SOP_Refresh_Timestamp)&amp;" "&amp;TEXT(SOP_Refresh_Timestamp,"HH:MM:SS"),"Offline")&amp;" | UoM: "&amp;IFERROR(SOP_TargetUoM,"(None)")&amp;" | Currency: "&amp;IFERROR(SOP_TargetCurrency,"(None)")</f>
         <v>Last Refresh: 1900-Jan-0 00:00:00 | UoM: (None) | Currency: (None)</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="42"/>
       <c r="L3" s="42"/>
       <c r="M3" s="42"/>
@@ -9853,8 +9853,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="5121" r:id="rId6" name="FPMExcelClientSheetOptionstb1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="5127" r:id="rId6" name="TextBox2">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
+            <anchor>
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="5127" r:id="rId6" name="TextBox2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="5121" r:id="rId8" name="FPMExcelClientSheetOptionstb1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -9873,32 +9898,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="5121" r:id="rId6" name="FPMExcelClientSheetOptionstb1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="5127" r:id="rId8" name="TextBox2">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId9">
-            <anchor>
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="5127" r:id="rId8" name="TextBox2"/>
+        <control shapeId="5121" r:id="rId8" name="FPMExcelClientSheetOptionstb1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>